<commit_message>
fuzesedu - update stretnutia
</commit_message>
<xml_diff>
--- a/USI cerny ukol - sraz.xlsx
+++ b/USI cerny ukol - sraz.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Docházka: (upravte text a barvu pozadí)</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Přidávejte časy a dny a vybarvěte pozadí jak kdo budete moci</t>
+  </si>
+  <si>
+    <t>celý den</t>
+  </si>
+  <si>
+    <t>18.10.</t>
+  </si>
+  <si>
+    <t>17.10.</t>
   </si>
 </sst>
 </file>
@@ -290,9 +299,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,9 +336,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -345,14 +354,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -390,9 +402,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,7 +439,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,7 +474,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -639,7 +651,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,306 +660,318 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="F14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="A17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="A18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>